<commit_message>
Updated Excel Spreadsheet with sources and specs
</commit_message>
<xml_diff>
--- a/DWGs, PDFs, XLS (Manifold)/Manifold Mass.xlsx
+++ b/DWGs, PDFs, XLS (Manifold)/Manifold Mass.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerse\Documents\GitHub\MECH-400-Team-4\DWGs, PDFs, XLS (Manifold)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan\Documents\GitHub\MECH-400-Team-4\DWGs, PDFs, XLS (Manifold)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557EFBB9-0722-4467-A33E-8E2F0C82C75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD261B36-9557-4362-8566-3CAC23A08B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Component</t>
   </si>
@@ -86,13 +86,40 @@
     <t>weight from another manufacturer since EPG had a 404 error, need their values</t>
   </si>
   <si>
-    <t>EPG</t>
-  </si>
-  <si>
     <t>Mazzei</t>
   </si>
   <si>
-    <t>Wolesely</t>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>12" DR17</t>
+  </si>
+  <si>
+    <t>12"x12"x6" DR17</t>
+  </si>
+  <si>
+    <t>6" DR17</t>
+  </si>
+  <si>
+    <t>EPG, IPS FAB TEE</t>
+  </si>
+  <si>
+    <t>EPG, IPS FAB BRANCH SADDLE RED. TEE</t>
+  </si>
+  <si>
+    <t>EPG, IPS FLANGE ADAPTER</t>
+  </si>
+  <si>
+    <t>Wolesely, IPS HDPE BLIND FLANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12" </t>
+  </si>
+  <si>
+    <t>EPG, PIPE CHART</t>
+  </si>
+  <si>
+    <t>N60-F PP</t>
   </si>
 </sst>
 </file>
@@ -469,23 +496,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,8 +532,11 @@
       <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -524,10 +555,13 @@
         <v>16.818181818181817</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -546,10 +580,13 @@
         <v>141.81818181818181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -568,10 +605,13 @@
         <v>155.45454545454544</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -589,11 +629,12 @@
         <f>D5/2.2</f>
         <v>231.45454545454544</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -612,10 +653,13 @@
         <v>11.818181818181817</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -635,10 +679,13 @@
         <v>74.039999999999978</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -657,10 +704,13 @@
         <v>18.18181818181818</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -678,11 +728,12 @@
         <f t="shared" si="1"/>
         <v>29.963636363636361</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -701,18 +752,22 @@
         <v>16.618181818181817</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -725,6 +780,7 @@
         <v>696.16727272727269</v>
       </c>
       <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>